<commit_message>
fix month in Unix Time
</commit_message>
<xml_diff>
--- a/Arduino/payload_decoder.xlsx
+++ b/Arduino/payload_decoder.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt\code\DistributedWaterLevelMonitor\Arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF1E1708-BCF3-428A-BE99-521D8D3F60DE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB92E29-DFBC-41AB-9928-7A03FD8A0A38}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{236FC34C-51CC-4A1E-9BF8-76C17D95DCA9}"/>
   </bookViews>
@@ -69,7 +69,7 @@
     <t>inHg Pressure</t>
   </si>
   <si>
-    <t>5E6E61190001008F088508900AC37707008F088508950AC177060090088508AC0AAF7707008F089108E20A677702</t>
+    <t>5e7fc9b0003c00e10219031e1bb470f100e3021f02f31be7710700e402a3037b197770c400e3032c03bb18a870ba</t>
   </si>
 </sst>
 </file>
@@ -77,7 +77,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="dd\/mm\/yy\ hh:mm"/>
+    <numFmt numFmtId="164" formatCode="dd\/mm\/yy\ hh:mm"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -115,10 +115,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,7 +436,7 @@
   <dimension ref="A1:AL11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="A2" sqref="A2:AL2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -450,71 +450,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
     </row>
     <row r="2" spans="1:38">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-      <c r="AC2" s="1"/>
-      <c r="AD2" s="1"/>
-      <c r="AE2" s="1"/>
-      <c r="AF2" s="1"/>
-      <c r="AG2" s="1"/>
-      <c r="AH2" s="1"/>
-      <c r="AI2" s="1"/>
-      <c r="AJ2" s="1"/>
-      <c r="AK2" s="1"/>
-      <c r="AL2" s="1"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2"/>
+      <c r="AG2" s="2"/>
+      <c r="AH2" s="2"/>
+      <c r="AI2" s="2"/>
+      <c r="AJ2" s="2"/>
+      <c r="AK2" s="2"/>
+      <c r="AL2" s="2"/>
     </row>
     <row r="3" spans="1:38">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <f>(((HEX2DEC(MID(A1, 1, 8))/60)/60/24)+DATE(1970,1,1))</f>
-        <v>43905.714363425926</v>
+        <v>43918.919074074074</v>
       </c>
     </row>
     <row r="4" spans="1:38">
@@ -523,7 +523,7 @@
       </c>
       <c r="B4">
         <f>HEX2DEC(MID(A1,9,4))</f>
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -546,28 +546,28 @@
     <row r="7" spans="1:38">
       <c r="A7">
         <f>HEX2DEC(MID(A1,13,4))</f>
-        <v>143</v>
+        <v>225</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7">
         <f>HEX2DEC(MID(A1,33,4))</f>
-        <v>143</v>
+        <v>227</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
       </c>
       <c r="E7">
         <f>HEX2DEC(MID(A1,53,4))</f>
-        <v>144</v>
+        <v>228</v>
       </c>
       <c r="F7" t="s">
         <v>7</v>
       </c>
       <c r="G7">
         <f>HEX2DEC(MID(A1,73,4))</f>
-        <v>143</v>
+        <v>227</v>
       </c>
       <c r="H7" t="s">
         <v>7</v>
@@ -576,28 +576,28 @@
     <row r="8" spans="1:38">
       <c r="A8">
         <f>HEX2DEC(MID(A1,17,4))/100</f>
-        <v>21.81</v>
+        <v>5.37</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8">
         <f>HEX2DEC(MID(A1,37,4))/100</f>
-        <v>21.81</v>
+        <v>5.43</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
       </c>
       <c r="E8">
         <f>HEX2DEC(MID(A1,57,4))/100</f>
-        <v>21.81</v>
+        <v>6.75</v>
       </c>
       <c r="F8" t="s">
         <v>8</v>
       </c>
       <c r="G8">
         <f>HEX2DEC(MID(A1,77,4))/100</f>
-        <v>21.93</v>
+        <v>8.1199999999999992</v>
       </c>
       <c r="H8" t="s">
         <v>8</v>
@@ -606,28 +606,28 @@
     <row r="9" spans="1:38">
       <c r="A9">
         <f>HEX2DEC(MID(A1,21,4))/100</f>
-        <v>21.92</v>
+        <v>7.98</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9">
         <f>HEX2DEC(MID(A1,41,4))/100</f>
-        <v>21.97</v>
+        <v>7.55</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
       </c>
       <c r="E9">
         <f>HEX2DEC(MID(A1,61,4))/100</f>
-        <v>22.2</v>
+        <v>8.91</v>
       </c>
       <c r="F9" t="s">
         <v>9</v>
       </c>
       <c r="G9">
         <f>HEX2DEC(MID(A1,81,4))/100</f>
-        <v>22.74</v>
+        <v>9.5500000000000007</v>
       </c>
       <c r="H9" t="s">
         <v>9</v>
@@ -636,28 +636,28 @@
     <row r="10" spans="1:38">
       <c r="A10">
         <f>HEX2DEC(MID(A1,25,4))/100</f>
-        <v>27.55</v>
+        <v>70.92</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10">
         <f>HEX2DEC(MID(A1,45,4))/100</f>
-        <v>27.53</v>
+        <v>71.430000000000007</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>
       </c>
       <c r="E10">
         <f>HEX2DEC(MID(A1,65,4))/100</f>
-        <v>27.35</v>
+        <v>65.19</v>
       </c>
       <c r="F10" t="s">
         <v>10</v>
       </c>
       <c r="G10">
         <f>HEX2DEC(MID(A1,85,4))/100</f>
-        <v>26.63</v>
+        <v>63.12</v>
       </c>
       <c r="H10" t="s">
         <v>10</v>
@@ -666,28 +666,28 @@
     <row r="11" spans="1:38">
       <c r="A11">
         <f>HEX2DEC(MID(A1,29,4))/1000</f>
-        <v>30.471</v>
+        <v>28.913</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11">
         <f>HEX2DEC(MID(A1,49,4))/1000</f>
-        <v>30.47</v>
+        <v>28.934999999999999</v>
       </c>
       <c r="D11" t="s">
         <v>11</v>
       </c>
       <c r="E11">
         <f>HEX2DEC(MID(A1,69,4))/1000</f>
-        <v>30.471</v>
+        <v>28.867999999999999</v>
       </c>
       <c r="F11" t="s">
         <v>11</v>
       </c>
       <c r="G11">
         <f>HEX2DEC(MID(A1,89,4))/1000</f>
-        <v>30.466000000000001</v>
+        <v>28.858000000000001</v>
       </c>
       <c r="H11" t="s">
         <v>11</v>

</xml_diff>